<commit_message>
#355 More ExcelSchemaBuilder feature implemented (see tests)
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9451913E-5F01-40B1-A57A-E93A82597DFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D68D928-5EA2-4A58-A9FB-43DF9755C01D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="3390" windowWidth="20580" windowHeight="11130" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4275" yWindow="1785" windowWidth="20580" windowHeight="11130" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="5" r:id="rId1"/>
@@ -18,13 +18,18 @@
     <sheet name="Multiplicity" sheetId="7" r:id="rId3"/>
     <sheet name="Range" sheetId="8" r:id="rId4"/>
     <sheet name="XSDExclusive" sheetId="9" r:id="rId5"/>
+    <sheet name="DefaultValue" sheetId="10" r:id="rId6"/>
+    <sheet name="Documentation" sheetId="11" r:id="rId7"/>
+    <sheet name="Values" sheetId="12" r:id="rId8"/>
+    <sheet name="Pattern" sheetId="13" r:id="rId9"/>
+    <sheet name="Digits" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -183,6 +188,54 @@
   </si>
   <si>
     <t>Multiplicity</t>
+  </si>
+  <si>
+    <t>DefaultValue</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>documentation</t>
+  </si>
+  <si>
+    <t>Field has Documentation</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>pattern</t>
+  </si>
+  <si>
+    <t>male|female</t>
+  </si>
+  <si>
+    <t>Digits</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>totalDigits</t>
+  </si>
+  <si>
+    <t>fractionDigits</t>
+  </si>
+  <si>
+    <t>male, female, she male</t>
   </si>
 </sst>
 </file>
@@ -1176,6 +1229,73 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD8192E-49C0-4792-991A-D63BBCDA3251}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1051FC8A-45FF-430E-806F-18C2C91AFA50}">
   <dimension ref="A1:C3"/>
@@ -1236,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C65980-0B1B-4CAD-8672-FF8AE8F17C37}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -1559,4 +1679,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BC5114-E86A-4509-9711-F7E3B127020F}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A9775B-918C-4A83-A4AE-FA22E877E548}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35032079-5C26-4C12-99C9-D449945A5E02}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287548FE-BF2B-47D2-9F17-07261DB3E72B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#355 attributes are implemented
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D68D928-5EA2-4A58-A9FB-43DF9755C01D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3EB894-240F-41F8-8CA6-873B6662D1B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="1785" windowWidth="20580" windowHeight="11130" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12103" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="5" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="Values" sheetId="12" r:id="rId8"/>
     <sheet name="Pattern" sheetId="13" r:id="rId9"/>
     <sheet name="Digits" sheetId="14" r:id="rId10"/>
+    <sheet name="Attribute" sheetId="15" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="73">
   <si>
     <t>name</t>
   </si>
@@ -236,6 +237,18 @@
   </si>
   <si>
     <t>male, female, she male</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>attribute</t>
   </si>
 </sst>
 </file>
@@ -1116,18 +1129,18 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="15.84375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" customWidth="1"/>
+    <col min="7" max="7" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1138,7 +1151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1146,7 +1159,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1157,7 +1170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1168,7 +1181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1179,7 +1192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1190,7 +1203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1201,7 +1214,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1212,7 +1225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1238,17 +1251,17 @@
       <selection pane="bottomLeft" activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="3" width="17.3828125" customWidth="1"/>
+    <col min="4" max="4" width="15.84375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" customWidth="1"/>
+    <col min="7" max="7" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1265,7 +1278,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1273,7 +1286,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1288,6 +1301,61 @@
       </c>
       <c r="E3">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E344D7-A53C-4373-BD98-318C6E4940A0}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="13.3828125" customWidth="1"/>
+    <col min="4" max="4" width="17.69140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1305,18 +1373,18 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="15.84375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" customWidth="1"/>
+    <col min="7" max="7" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1327,7 +1395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1335,7 +1403,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1361,15 +1429,15 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="13.3828125" customWidth="1"/>
+    <col min="4" max="4" width="12.15234375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1383,7 +1451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1394,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1402,7 +1470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1492,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1435,7 +1503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1514,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1472,14 +1540,14 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="3" width="17.3828125" customWidth="1"/>
+    <col min="4" max="4" width="12.15234375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1493,7 +1561,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1501,7 +1569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1515,7 +1583,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1529,7 +1597,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1543,7 +1611,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1572,17 +1640,17 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1605,7 +1673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1613,7 +1681,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1630,7 +1698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1647,7 +1715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1661,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1690,18 +1758,18 @@
       <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" customWidth="1"/>
+    <col min="4" max="4" width="15.84375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.3828125" customWidth="1"/>
+    <col min="7" max="7" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1715,7 +1783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1791,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1752,17 +1820,17 @@
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="23.3828125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.3828125" customWidth="1"/>
+    <col min="6" max="6" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1773,7 +1841,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1781,7 +1849,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1802,22 +1870,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35032079-5C26-4C12-99C9-D449945A5E02}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.3828125" customWidth="1"/>
+    <col min="6" max="6" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1828,7 +1896,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1836,7 +1904,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1862,17 +1930,17 @@
       <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.84375" customWidth="1"/>
+    <col min="2" max="2" width="17.3828125" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.3828125" customWidth="1"/>
+    <col min="6" max="6" width="17.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1883,7 +1951,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1891,7 +1959,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
#410 TabularSchemaBuilder use xsd sequence by default
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmyt\workspace\cristal-ise\dsl\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A6120-D17F-4C2B-9A74-C35D57E86CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D4AAD4-1DA4-4C6A-A8EC-49BC3FF5D50C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="2955" windowWidth="18900" windowHeight="11100" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>name</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>xsd</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -774,7 +777,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -783,6 +786,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1160,11 +1164,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1291,13 +1295,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1368,10 +1372,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1420,7 +1424,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,16 +1438,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1524,11 +1528,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1575,7 +1579,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,12 +1591,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1693,29 +1697,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CA0F3F-D6D3-4156-AD15-7844900A3854}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1725,19 +1731,25 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1747,11 +1759,11 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1761,11 +1773,11 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1775,11 +1787,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1789,13 +1801,13 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1822,15 +1834,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1955,12 +1967,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2027,11 +2039,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2092,11 +2104,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2157,11 +2169,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
Fixing generated Schema test with generated PredefiendSteps anyType
</commit_message>
<xml_diff>
--- a/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
+++ b/dsl/src/test/data/ExcelSchemaBuilderField.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="83">
   <si>
     <t xml:space="preserve">xsd</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t xml:space="preserve">dateTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anyTypeField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anyType</t>
   </si>
   <si>
     <t xml:space="preserve">UnknownType</t>
@@ -401,12 +407,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,6 +528,17 @@
       </c>
       <c r="C10" s="0" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -582,10 +599,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,7 +618,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>14</v>
@@ -668,7 +685,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,15 +693,15 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -733,7 +750,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -748,13 +765,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -774,16 +791,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -808,7 +825,7 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -837,7 +854,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,7 +862,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,14 +870,14 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="str">
         <f aca="false">E4</f>
         <v>male, female, she male</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -868,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C5" s="0" t="str">
         <f aca="false">UnitWithValues!E1</f>
@@ -938,7 +955,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,10 +963,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1004,10 +1021,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,7 +1032,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -1027,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,10 +1052,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>500</v>
@@ -1057,10 +1074,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,10 +1085,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,10 +1096,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1141,10 +1158,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,10 +1169,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,13 +1180,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,13 +1194,13 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,13 +1208,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1205,13 +1222,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1275,16 +1292,16 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,7 +1309,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,7 +1317,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>12</v>
@@ -1317,7 +1334,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>12</v>
@@ -1334,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>12</v>
@@ -1348,7 +1365,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>12</v>
@@ -1415,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,7 +1440,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,13 +1448,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1493,7 +1510,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1501,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1512,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1568,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,7 +1593,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,10 +1601,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1643,7 +1660,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1651,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,10 +1676,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>